<commit_message>
Max stat collection part 2
</commit_message>
<xml_diff>
--- a/0_10_all.xlsx
+++ b/0_10_all.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -521,10 +521,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -846,15 +847,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -891,8 +892,44 @@
       <c r="L1">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>20</v>
+      </c>
+      <c r="R1" s="3">
+        <v>30</v>
+      </c>
+      <c r="S1" s="3">
+        <v>40</v>
+      </c>
+      <c r="T1" s="3">
+        <v>50</v>
+      </c>
+      <c r="U1" s="3">
+        <v>60</v>
+      </c>
+      <c r="V1" s="3">
+        <v>70</v>
+      </c>
+      <c r="W1" s="3">
+        <v>80</v>
+      </c>
+      <c r="X1" s="3">
+        <v>90</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>100</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -929,8 +966,44 @@
       <c r="L2" s="1">
         <v>5.8077485380117002</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>4.1071428571428603</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>4.3846153846153904</v>
+      </c>
+      <c r="R2" s="3">
+        <v>4.7916666666666696</v>
+      </c>
+      <c r="S2" s="3">
+        <v>4.9130434782608701</v>
+      </c>
+      <c r="T2" s="3">
+        <v>5.3333333333333304</v>
+      </c>
+      <c r="U2" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="V2" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="W2" s="3">
+        <v>5.55</v>
+      </c>
+      <c r="X2" s="3">
+        <v>5.5263157894736796</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>5.9473684210526301</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>5.8947368421052602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -967,8 +1040,44 @@
       <c r="L3">
         <v>5.3676641830821401</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O3" s="3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="3">
+        <v>3.9655172413793101</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R3" s="2">
+        <v>5</v>
+      </c>
+      <c r="S3" s="3">
+        <v>5</v>
+      </c>
+      <c r="T3" s="3">
+        <v>5.375</v>
+      </c>
+      <c r="U3" s="3">
+        <v>5.4444444444444402</v>
+      </c>
+      <c r="V3" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="W3" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="X3" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>5.8947368421052602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1005,8 +1114,44 @@
       <c r="L4">
         <v>5.5926384588923304</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O4" s="3">
+        <v>2</v>
+      </c>
+      <c r="P4" s="3">
+        <v>3.9655172413793101</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R4" s="2">
+        <v>5</v>
+      </c>
+      <c r="S4" s="2">
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="T4" s="3">
+        <v>5.3333333333333304</v>
+      </c>
+      <c r="U4" s="3">
+        <v>5.4736842105263204</v>
+      </c>
+      <c r="V4" s="3">
+        <v>5.4285714285714297</v>
+      </c>
+      <c r="W4" s="3">
+        <v>5.6666666666666696</v>
+      </c>
+      <c r="X4" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1043,44 +1188,44 @@
       <c r="L5">
         <v>5.5125631102643498</v>
       </c>
-      <c r="Q5" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>10</v>
-      </c>
-      <c r="S5">
-        <v>20</v>
-      </c>
-      <c r="T5">
-        <v>30</v>
-      </c>
-      <c r="U5">
-        <v>40</v>
-      </c>
-      <c r="V5">
-        <v>50</v>
-      </c>
-      <c r="W5">
-        <v>60</v>
-      </c>
-      <c r="X5">
-        <v>70</v>
-      </c>
-      <c r="Y5">
-        <v>80</v>
-      </c>
-      <c r="Z5">
-        <v>90</v>
-      </c>
-      <c r="AA5">
-        <v>100</v>
-      </c>
-      <c r="AB5">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O5" s="3">
+        <v>3</v>
+      </c>
+      <c r="P5" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R5" s="3">
+        <v>4.8695652173913002</v>
+      </c>
+      <c r="S5" s="3">
+        <v>5</v>
+      </c>
+      <c r="T5" s="3">
+        <v>5.3809523809523796</v>
+      </c>
+      <c r="U5" s="3">
+        <v>5.4285714285714297</v>
+      </c>
+      <c r="V5" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="W5" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="X5" s="3">
+        <v>5.6666666666666696</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>5.7894736842105301</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1117,8 +1262,44 @@
       <c r="L6">
         <v>5.63650541795666</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O6" s="3">
+        <v>4</v>
+      </c>
+      <c r="P6" s="3">
+        <v>3.84</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R6" s="2">
+        <v>5</v>
+      </c>
+      <c r="S6" s="3">
+        <v>5</v>
+      </c>
+      <c r="T6" s="3">
+        <v>5.375</v>
+      </c>
+      <c r="U6" s="3">
+        <v>5.4285714285714297</v>
+      </c>
+      <c r="V6" s="3">
+        <v>5.2272727272727302</v>
+      </c>
+      <c r="W6" s="2">
+        <v>5.8888888888888902</v>
+      </c>
+      <c r="X6" s="2">
+        <v>5.8888888888888902</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>5.9444444444444402</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>5.9444444444444402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1155,8 +1336,44 @@
       <c r="L7">
         <v>5.5568249054007604</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O7" s="3">
+        <v>5</v>
+      </c>
+      <c r="P7" s="3">
+        <v>3.7666666666666702</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R7" s="3">
+        <v>4.7826086956521703</v>
+      </c>
+      <c r="S7" s="3">
+        <v>5.1363636363636402</v>
+      </c>
+      <c r="T7" s="3">
+        <v>5.3809523809523796</v>
+      </c>
+      <c r="U7" s="3">
+        <v>5.4761904761904798</v>
+      </c>
+      <c r="V7" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="W7" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="X7" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>5.6666666666666696</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>5.9473684210526301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1193,8 +1410,44 @@
       <c r="L8">
         <v>5.4792295784710703</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O8" s="3">
+        <v>6</v>
+      </c>
+      <c r="P8" s="3">
+        <v>3.9655172413793101</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>4.3461538461538503</v>
+      </c>
+      <c r="R8" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="S8" s="3">
+        <v>5</v>
+      </c>
+      <c r="T8" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="U8" s="3">
+        <v>5.4285714285714297</v>
+      </c>
+      <c r="V8" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="W8" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X8" s="3">
+        <v>5.6666666666666696</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>5.6666666666666696</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1231,8 +1484,44 @@
       <c r="L9">
         <v>5.5569298245613998</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O9" s="3">
+        <v>7</v>
+      </c>
+      <c r="P9" s="3">
+        <v>4.1481481481481497</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R9" s="2">
+        <v>5</v>
+      </c>
+      <c r="S9" s="3">
+        <v>5.1363636363636402</v>
+      </c>
+      <c r="T9" s="3">
+        <v>5.375</v>
+      </c>
+      <c r="U9" s="3">
+        <v>5.4444444444444402</v>
+      </c>
+      <c r="V9" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="W9" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X9" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1269,8 +1558,44 @@
       <c r="L10">
         <v>5.5805323357413101</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O10" s="3">
+        <v>8</v>
+      </c>
+      <c r="P10" s="3">
+        <v>4.0625</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R10" s="3">
+        <v>4.7916666666666696</v>
+      </c>
+      <c r="S10" s="3">
+        <v>5.05</v>
+      </c>
+      <c r="T10" s="3">
+        <v>5.2272727272727302</v>
+      </c>
+      <c r="U10" s="3">
+        <v>5.4285714285714297</v>
+      </c>
+      <c r="V10" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="W10" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X10" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>5.9411764705882399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1307,8 +1632,44 @@
       <c r="L11">
         <v>5.43908873805933</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O11" s="3">
+        <v>9</v>
+      </c>
+      <c r="P11" s="3">
+        <v>4.0416666666666696</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R11" s="2">
+        <v>5</v>
+      </c>
+      <c r="S11" s="2">
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="T11" s="3">
+        <v>5.2272727272727302</v>
+      </c>
+      <c r="U11" s="3">
+        <v>5.2272727272727302</v>
+      </c>
+      <c r="V11" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="W11" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="X11" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>5.7647058823529402</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1345,8 +1706,44 @@
       <c r="L12">
         <v>5.5170269423558898</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O12" s="3">
+        <v>10</v>
+      </c>
+      <c r="P12" s="3">
+        <v>4.07407407407407</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>4.2592592592592604</v>
+      </c>
+      <c r="R12" s="3">
+        <v>4.7916666666666696</v>
+      </c>
+      <c r="S12" s="3">
+        <v>5</v>
+      </c>
+      <c r="T12" s="3">
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="U12" s="3">
+        <v>5.2272727272727302</v>
+      </c>
+      <c r="V12" s="2">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="W12" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="X12" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>5.7647058823529402</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>5.7222222222222197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1394,8 +1791,55 @@
         <f t="shared" si="0"/>
         <v>5.8077485380117002</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="3">
+        <f>MAX(P2:P12)</f>
+        <v>4.2</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" ref="Q13" si="1">MAX(Q2:Q12)</f>
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R13" s="3">
+        <f t="shared" ref="R13" si="2">MAX(R2:R12)</f>
+        <v>5</v>
+      </c>
+      <c r="S13" s="3">
+        <f t="shared" ref="S13" si="3">MAX(S2:S12)</f>
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="T13" s="3">
+        <f t="shared" ref="T13" si="4">MAX(T2:T12)</f>
+        <v>5.6</v>
+      </c>
+      <c r="U13" s="3">
+        <f t="shared" ref="U13" si="5">MAX(U2:U12)</f>
+        <v>5.6</v>
+      </c>
+      <c r="V13" s="3">
+        <f t="shared" ref="V13" si="6">MAX(V2:V12)</f>
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="W13" s="3">
+        <f t="shared" ref="W13" si="7">MAX(W2:W12)</f>
+        <v>5.8888888888888902</v>
+      </c>
+      <c r="X13" s="3">
+        <f t="shared" ref="X13" si="8">MAX(X2:X12)</f>
+        <v>5.8888888888888902</v>
+      </c>
+      <c r="Y13" s="3">
+        <f t="shared" ref="Y13" si="9">MAX(Y2:Y12)</f>
+        <v>5.9473684210526301</v>
+      </c>
+      <c r="Z13" s="3">
+        <f t="shared" ref="Z13" si="10">MAX(Z2:Z12)</f>
+        <v>5.9473684210526301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1432,8 +1876,44 @@
       <c r="L15" s="2">
         <v>5.8289473684210504</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O15" s="3">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
+        <v>4.3461538461538503</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>4.3846153846153904</v>
+      </c>
+      <c r="R15" s="2">
+        <v>5.0909090909090899</v>
+      </c>
+      <c r="S15" s="3">
+        <v>4.8695652173913002</v>
+      </c>
+      <c r="T15" s="3">
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="U15" s="2">
+        <v>5.5625</v>
+      </c>
+      <c r="V15" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="W15" s="3">
+        <v>5.7894736842105301</v>
+      </c>
+      <c r="X15" s="3">
+        <v>5.5789473684210504</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>5.8947368421052602</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>5.9473684210526301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1470,8 +1950,44 @@
       <c r="L16">
         <v>5.3807516339869297</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O16" s="3">
+        <v>1</v>
+      </c>
+      <c r="P16" s="2">
+        <v>4.3846153846153904</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R16" s="3">
+        <v>5</v>
+      </c>
+      <c r="S16" s="3">
+        <v>5.0909090909090899</v>
+      </c>
+      <c r="T16" s="3">
+        <v>5.3809523809523796</v>
+      </c>
+      <c r="U16" s="3">
+        <v>5.4761904761904798</v>
+      </c>
+      <c r="V16" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="W16" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="X16" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>5.6470588235294104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1508,8 +2024,44 @@
       <c r="L17">
         <v>5.5780254557963502</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O17" s="3">
+        <v>2</v>
+      </c>
+      <c r="P17" s="3">
+        <v>4.2222222222222197</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="R17" s="3">
+        <v>5</v>
+      </c>
+      <c r="S17" s="3">
+        <v>5</v>
+      </c>
+      <c r="T17" s="3">
+        <v>5.3333333333333304</v>
+      </c>
+      <c r="U17" s="3">
+        <v>5.3809523809523796</v>
+      </c>
+      <c r="V17" s="2">
+        <v>5.75</v>
+      </c>
+      <c r="W17" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X17" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>5.5555555555555598</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1546,8 +2098,44 @@
       <c r="L18">
         <v>5.3823529411764701</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O18" s="3">
+        <v>3</v>
+      </c>
+      <c r="P18" s="3">
+        <v>4.1071428571428603</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R18" s="3">
+        <v>5</v>
+      </c>
+      <c r="S18" s="3">
+        <v>4.9565217391304301</v>
+      </c>
+      <c r="T18" s="3">
+        <v>5.3809523809523796</v>
+      </c>
+      <c r="U18" s="3">
+        <v>5.4761904761904798</v>
+      </c>
+      <c r="V18" s="3">
+        <v>5.4285714285714297</v>
+      </c>
+      <c r="W18" s="3">
+        <v>5.6842105263157903</v>
+      </c>
+      <c r="X18" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1584,8 +2172,44 @@
       <c r="L19">
         <v>5.5399465811965802</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O19" s="3">
+        <v>4</v>
+      </c>
+      <c r="P19" s="3">
+        <v>4.1071428571428603</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R19" s="3">
+        <v>5</v>
+      </c>
+      <c r="S19" s="3">
+        <v>5.1363636363636402</v>
+      </c>
+      <c r="T19" s="3">
+        <v>5.375</v>
+      </c>
+      <c r="U19" s="3">
+        <v>5.3333333333333304</v>
+      </c>
+      <c r="V19" s="3">
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="W19" s="2">
+        <v>5.8888888888888902</v>
+      </c>
+      <c r="X19" s="2">
+        <v>5.9444444444444402</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>5.9444444444444402</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>6.1666666666666696</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1622,8 +2246,44 @@
       <c r="L20">
         <v>5.4745734434124502</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O20" s="3">
+        <v>5</v>
+      </c>
+      <c r="P20" s="3">
+        <v>4.1851851851851896</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R20" s="3">
+        <v>5</v>
+      </c>
+      <c r="S20" s="3">
+        <v>5.0909090909090899</v>
+      </c>
+      <c r="T20" s="3">
+        <v>5.3333333333333304</v>
+      </c>
+      <c r="U20" s="3">
+        <v>5.3333333333333304</v>
+      </c>
+      <c r="V20" s="3">
+        <v>5.4444444444444402</v>
+      </c>
+      <c r="W20" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X20" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>5.6666666666666696</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -1660,8 +2320,44 @@
       <c r="L21">
         <v>5.5018894048847597</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O21" s="3">
+        <v>6</v>
+      </c>
+      <c r="P21" s="3">
+        <v>4.2307692307692299</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>4.3461538461538503</v>
+      </c>
+      <c r="R21" s="3">
+        <v>5</v>
+      </c>
+      <c r="S21" s="3">
+        <v>5</v>
+      </c>
+      <c r="T21" s="3">
+        <v>5.3809523809523796</v>
+      </c>
+      <c r="U21" s="3">
+        <v>5.4761904761904798</v>
+      </c>
+      <c r="V21" s="2">
+        <v>5.75</v>
+      </c>
+      <c r="W21" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X21" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1698,8 +2394,44 @@
       <c r="L22">
         <v>5.4533436532507702</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O22" s="3">
+        <v>7</v>
+      </c>
+      <c r="P22" s="3">
+        <v>4.1481481481481497</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="R22" s="3">
+        <v>4.7916666666666696</v>
+      </c>
+      <c r="S22" s="3">
+        <v>5.1363636363636402</v>
+      </c>
+      <c r="T22" s="2">
+        <v>5.3809523809523796</v>
+      </c>
+      <c r="U22" s="3">
+        <v>5.3333333333333304</v>
+      </c>
+      <c r="V22" s="3">
+        <v>5.4285714285714297</v>
+      </c>
+      <c r="W22" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X22" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1736,8 +2468,44 @@
       <c r="L23">
         <v>5.4782645338837304</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O23" s="3">
+        <v>8</v>
+      </c>
+      <c r="P23" s="3">
+        <v>3.9310344827586201</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R23" s="3">
+        <v>5</v>
+      </c>
+      <c r="S23" s="3">
+        <v>5</v>
+      </c>
+      <c r="T23" s="3">
+        <v>5.3333333333333304</v>
+      </c>
+      <c r="U23" s="3">
+        <v>5.4444444444444402</v>
+      </c>
+      <c r="V23" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="W23" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X23" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>5.5555555555555598</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>5.875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -1774,8 +2542,44 @@
       <c r="L24">
         <v>5.4071207430340502</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O24" s="3">
+        <v>9</v>
+      </c>
+      <c r="P24" s="3">
+        <v>4.0714285714285703</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R24" s="3">
+        <v>4.9565217391304301</v>
+      </c>
+      <c r="S24" s="2">
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="T24" s="3">
+        <v>5.2666666666666702</v>
+      </c>
+      <c r="U24" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="V24" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="W24" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+      <c r="X24" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -1812,8 +2616,44 @@
       <c r="L25">
         <v>5.4633603238866399</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O25" s="3">
+        <v>10</v>
+      </c>
+      <c r="P25" s="3">
+        <v>4.1071428571428603</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>4.4230769230769198</v>
+      </c>
+      <c r="R25" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="S25" s="3">
+        <v>5.1363636363636402</v>
+      </c>
+      <c r="T25" s="3">
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="U25" s="3">
+        <v>5.4761904761904798</v>
+      </c>
+      <c r="V25" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="W25" s="3">
+        <v>5.875</v>
+      </c>
+      <c r="X25" s="3">
+        <v>5.6666666666666696</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>5.8421052631578902</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1826,40 +2666,638 @@
         <v>4.3688408628408597</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26" si="1">MAX(D15:D25)</f>
+        <f t="shared" ref="D26" si="11">MAX(D15:D25)</f>
         <v>4.6446153846153804</v>
       </c>
       <c r="E26">
-        <f t="shared" ref="E26" si="2">MAX(E15:E25)</f>
+        <f t="shared" ref="E26" si="12">MAX(E15:E25)</f>
         <v>4.76718426501035</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F26" si="3">MAX(F15:F25)</f>
+        <f t="shared" ref="F26" si="13">MAX(F15:F25)</f>
         <v>5.0713344626388102</v>
       </c>
       <c r="G26">
-        <f t="shared" ref="G26" si="4">MAX(G15:G25)</f>
+        <f t="shared" ref="G26" si="14">MAX(G15:G25)</f>
         <v>5.1606744133059896</v>
       </c>
       <c r="H26">
-        <f t="shared" ref="H26" si="5">MAX(H15:H25)</f>
+        <f t="shared" ref="H26" si="15">MAX(H15:H25)</f>
         <v>5.3793939393939398</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I26" si="6">MAX(I15:I25)</f>
+        <f t="shared" ref="I26" si="16">MAX(I15:I25)</f>
         <v>5.4154360500180898</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26" si="7">MAX(J15:J25)</f>
+        <f t="shared" ref="J26" si="17">MAX(J15:J25)</f>
         <v>5.5676169590643303</v>
       </c>
       <c r="K26">
-        <f t="shared" ref="K26" si="8">MAX(K15:K25)</f>
+        <f t="shared" ref="K26" si="18">MAX(K15:K25)</f>
         <v>5.7867905056759597</v>
       </c>
       <c r="L26">
-        <f t="shared" ref="L26" si="9">MAX(L15:L25)</f>
+        <f t="shared" ref="L26" si="19">MAX(L15:L25)</f>
         <v>5.8289473684210504</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P26" s="3">
+        <f>MAX(P15:P25)</f>
+        <v>4.3846153846153904</v>
+      </c>
+      <c r="Q26" s="3">
+        <f t="shared" ref="Q26" si="20">MAX(Q15:Q25)</f>
+        <v>4.5</v>
+      </c>
+      <c r="R26" s="3">
+        <f t="shared" ref="R26" si="21">MAX(R15:R25)</f>
+        <v>5.0909090909090899</v>
+      </c>
+      <c r="S26" s="3">
+        <f t="shared" ref="S26" si="22">MAX(S15:S25)</f>
+        <v>5.1818181818181799</v>
+      </c>
+      <c r="T26" s="3">
+        <f t="shared" ref="T26" si="23">MAX(T15:T25)</f>
+        <v>5.3809523809523796</v>
+      </c>
+      <c r="U26" s="3">
+        <f t="shared" ref="U26" si="24">MAX(U15:U25)</f>
+        <v>5.5625</v>
+      </c>
+      <c r="V26" s="3">
+        <f t="shared" ref="V26" si="25">MAX(V15:V25)</f>
+        <v>5.75</v>
+      </c>
+      <c r="W26" s="3">
+        <f t="shared" ref="W26" si="26">MAX(W15:W25)</f>
+        <v>5.8888888888888902</v>
+      </c>
+      <c r="X26" s="3">
+        <f t="shared" ref="X26" si="27">MAX(X15:X25)</f>
+        <v>5.9444444444444402</v>
+      </c>
+      <c r="Y26" s="3">
+        <f t="shared" ref="Y26" si="28">MAX(Y15:Y25)</f>
+        <v>5.9444444444444402</v>
+      </c>
+      <c r="Z26" s="3">
+        <f t="shared" ref="Z26" si="29">MAX(Z15:Z25)</f>
+        <v>6.1666666666666696</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>0</v>
+      </c>
+      <c r="B28" s="3">
+        <v>3.4520258159414801</v>
+      </c>
+      <c r="C28" s="3">
+        <v>4.0681318681318697</v>
+      </c>
+      <c r="D28" s="3">
+        <v>4.4956884057971003</v>
+      </c>
+      <c r="E28" s="3">
+        <v>4.6826581027668004</v>
+      </c>
+      <c r="F28" s="3">
+        <v>4.9534396762657602</v>
+      </c>
+      <c r="G28" s="2">
+        <v>5.1990720873329597</v>
+      </c>
+      <c r="H28" s="3">
+        <v>5.3137229437229401</v>
+      </c>
+      <c r="I28" s="3">
+        <v>5.4164411027568899</v>
+      </c>
+      <c r="J28" s="3">
+        <v>5.43762740183793</v>
+      </c>
+      <c r="K28" s="2">
+        <v>5.2913689526847403</v>
+      </c>
+      <c r="L28" s="2">
+        <v>5.7147243107769397</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3">
+        <v>3.51905974949389</v>
+      </c>
+      <c r="C29" s="3">
+        <v>4.0182336182336202</v>
+      </c>
+      <c r="D29" s="3">
+        <v>4.5063266443701204</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4.7962285902503297</v>
+      </c>
+      <c r="F29" s="3">
+        <v>4.8646527385657796</v>
+      </c>
+      <c r="G29" s="3">
+        <v>5.0883714473931896</v>
+      </c>
+      <c r="H29" s="2">
+        <v>5.3132756132756098</v>
+      </c>
+      <c r="I29" s="2">
+        <v>5.4921085858585901</v>
+      </c>
+      <c r="J29" s="3">
+        <v>5.4714202172096904</v>
+      </c>
+      <c r="K29" s="3">
+        <v>5.4938387635756003</v>
+      </c>
+      <c r="L29" s="3">
+        <v>5.2316489753796303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3">
+        <v>3.7080864560654598</v>
+      </c>
+      <c r="C30" s="3">
+        <v>4.2713675213675204</v>
+      </c>
+      <c r="D30" s="3">
+        <v>4.5252435897435896</v>
+      </c>
+      <c r="E30" s="3">
+        <v>4.8158662714097504</v>
+      </c>
+      <c r="F30" s="3">
+        <v>4.9305900621117997</v>
+      </c>
+      <c r="G30" s="3">
+        <v>4.9966647844908696</v>
+      </c>
+      <c r="H30" s="3">
+        <v>5.11944371799063</v>
+      </c>
+      <c r="I30" s="3">
+        <v>5.3763047770942496</v>
+      </c>
+      <c r="J30" s="3">
+        <v>5.4285021376971798</v>
+      </c>
+      <c r="K30" s="3">
+        <v>5.4005929038282003</v>
+      </c>
+      <c r="L30" s="3">
+        <v>5.5258496732026101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>3</v>
+      </c>
+      <c r="B31" s="3">
+        <v>3.6245242500825099</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4.3444444444444397</v>
+      </c>
+      <c r="D31" s="3">
+        <v>4.5317051282051297</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4.7613590250329398</v>
+      </c>
+      <c r="F31" s="3">
+        <v>4.9993388857519303</v>
+      </c>
+      <c r="G31" s="3">
+        <v>5.0125000000000002</v>
+      </c>
+      <c r="H31" s="3">
+        <v>5.2185630743525504</v>
+      </c>
+      <c r="I31" s="3">
+        <v>5.34114557226399</v>
+      </c>
+      <c r="J31" s="3">
+        <v>5.3959022556390996</v>
+      </c>
+      <c r="K31" s="3">
+        <v>5.3319504643962796</v>
+      </c>
+      <c r="L31" s="3">
+        <v>5.6397058823529402</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2">
+        <v>3.7758155151814798</v>
+      </c>
+      <c r="C32" s="3">
+        <v>4.2213675213675197</v>
+      </c>
+      <c r="D32" s="2">
+        <v>4.6261304347826098</v>
+      </c>
+      <c r="E32" s="3">
+        <v>4.6772318840579699</v>
+      </c>
+      <c r="F32" s="3">
+        <v>4.7544842838321104</v>
+      </c>
+      <c r="G32" s="3">
+        <v>4.9130059585723203</v>
+      </c>
+      <c r="H32" s="3">
+        <v>5.0975324675324698</v>
+      </c>
+      <c r="I32" s="3">
+        <v>5.0428947368421104</v>
+      </c>
+      <c r="J32" s="3">
+        <v>5.3619811784362899</v>
+      </c>
+      <c r="K32" s="3">
+        <v>5.6918885448916399</v>
+      </c>
+      <c r="L32" s="3">
+        <v>5.6053594771241801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>5</v>
+      </c>
+      <c r="B33" s="3">
+        <v>3.63286869870644</v>
+      </c>
+      <c r="C33" s="3">
+        <v>4.05783475783476</v>
+      </c>
+      <c r="D33" s="3">
+        <v>4.37692307692308</v>
+      </c>
+      <c r="E33" s="3">
+        <v>4.68034782608696</v>
+      </c>
+      <c r="F33" s="3">
+        <v>4.9680335968379401</v>
+      </c>
+      <c r="G33" s="3">
+        <v>5.1427272727272699</v>
+      </c>
+      <c r="H33" s="3">
+        <v>5.2383116883116898</v>
+      </c>
+      <c r="I33" s="3">
+        <v>5.39547103051747</v>
+      </c>
+      <c r="J33" s="3">
+        <v>5.3806643502696101</v>
+      </c>
+      <c r="K33" s="3">
+        <v>5.5195780561028203</v>
+      </c>
+      <c r="L33" s="3">
+        <v>5.4521695169295796</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>6</v>
+      </c>
+      <c r="B34" s="3">
+        <v>3.6885126367627801</v>
+      </c>
+      <c r="C34" s="3">
+        <v>4.1233618233618197</v>
+      </c>
+      <c r="D34" s="3">
+        <v>4.2658461538461498</v>
+      </c>
+      <c r="E34" s="3">
+        <v>4.7530580723624203</v>
+      </c>
+      <c r="F34" s="3">
+        <v>4.8287761151891599</v>
+      </c>
+      <c r="G34" s="3">
+        <v>5.0801399084007803</v>
+      </c>
+      <c r="H34" s="3">
+        <v>5.2146529201792404</v>
+      </c>
+      <c r="I34" s="3">
+        <v>5.3172964273428702</v>
+      </c>
+      <c r="J34" s="3">
+        <v>5.4356850459482002</v>
+      </c>
+      <c r="K34" s="3">
+        <v>5.5977837977296199</v>
+      </c>
+      <c r="L34" s="3">
+        <v>5.4478735677806904</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3">
+        <v>3.6382378702540001</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4.2445868945868899</v>
+      </c>
+      <c r="D35" s="3">
+        <v>4.4325256410256397</v>
+      </c>
+      <c r="E35" s="3">
+        <v>4.74537185354691</v>
+      </c>
+      <c r="F35" s="3">
+        <v>4.9527545642763</v>
+      </c>
+      <c r="G35" s="3">
+        <v>5.0305844155844204</v>
+      </c>
+      <c r="H35" s="3">
+        <v>5.2569696969697004</v>
+      </c>
+      <c r="I35" s="3">
+        <v>5.3700374041163501</v>
+      </c>
+      <c r="J35" s="3">
+        <v>5.4683800186741403</v>
+      </c>
+      <c r="K35" s="3">
+        <v>5.3946207430340598</v>
+      </c>
+      <c r="L35" s="3">
+        <v>5.5306372549019596</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>8</v>
+      </c>
+      <c r="B36" s="3">
+        <v>3.4963004312465298</v>
+      </c>
+      <c r="C36" s="3">
+        <v>4.2444444444444498</v>
+      </c>
+      <c r="D36" s="3">
+        <v>4.5123846153846197</v>
+      </c>
+      <c r="E36" s="3">
+        <v>4.8007608695652202</v>
+      </c>
+      <c r="F36" s="3">
+        <v>4.7295689817428901</v>
+      </c>
+      <c r="G36" s="3">
+        <v>5.0928627893845304</v>
+      </c>
+      <c r="H36" s="3">
+        <v>5.1942272347535496</v>
+      </c>
+      <c r="I36" s="3">
+        <v>5.4764745196324096</v>
+      </c>
+      <c r="J36" s="2">
+        <v>5.6094883040935697</v>
+      </c>
+      <c r="K36" s="3">
+        <v>5.4350303454715201</v>
+      </c>
+      <c r="L36" s="3">
+        <v>5.5052792142497999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>9</v>
+      </c>
+      <c r="B37" s="3">
+        <v>3.5516071488763399</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4.32877492877493</v>
+      </c>
+      <c r="D37" s="3">
+        <v>4.4902998885172796</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4.8541666666666696</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5.0718050065876197</v>
+      </c>
+      <c r="G37" s="3">
+        <v>5.1028780944456003</v>
+      </c>
+      <c r="H37" s="3">
+        <v>5.1203992193923504</v>
+      </c>
+      <c r="I37" s="3">
+        <v>5.2138816738816702</v>
+      </c>
+      <c r="J37" s="3">
+        <v>5.4697932330827097</v>
+      </c>
+      <c r="K37" s="3">
+        <v>5.4726143790849697</v>
+      </c>
+      <c r="L37" s="3">
+        <v>5.5356535947712402</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>10</v>
+      </c>
+      <c r="B38" s="3">
+        <v>3.5320352881267798</v>
+      </c>
+      <c r="C38" s="3">
+        <v>4.1183760683760697</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4.5527564102564098</v>
+      </c>
+      <c r="E38" s="3">
+        <v>4.5603333333333298</v>
+      </c>
+      <c r="F38" s="2">
+        <v>5.0110954263128198</v>
+      </c>
+      <c r="G38" s="3">
+        <v>5.08677771503858</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5.2777762092979499</v>
+      </c>
+      <c r="I38" s="3">
+        <v>5.1728654970760202</v>
+      </c>
+      <c r="J38" s="3">
+        <v>5.4429072681704298</v>
+      </c>
+      <c r="K38" s="3">
+        <v>5.5383333333333304</v>
+      </c>
+      <c r="L38" s="3">
+        <v>5.4900854700854698</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3">
+        <f>MAX(B28:B38)</f>
+        <v>3.7758155151814798</v>
+      </c>
+      <c r="C39" s="3">
+        <f>MAX(C28:C38)</f>
+        <v>4.3444444444444397</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" ref="D39" si="30">MAX(D28:D38)</f>
+        <v>4.6261304347826098</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" ref="E39" si="31">MAX(E28:E38)</f>
+        <v>4.8541666666666696</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" ref="F39" si="32">MAX(F28:F38)</f>
+        <v>5.0718050065876197</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" ref="G39" si="33">MAX(G28:G38)</f>
+        <v>5.1990720873329597</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" ref="H39" si="34">MAX(H28:H38)</f>
+        <v>5.3137229437229401</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" ref="I39" si="35">MAX(I28:I38)</f>
+        <v>5.4921085858585901</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" ref="J39" si="36">MAX(J28:J38)</f>
+        <v>5.6094883040935697</v>
+      </c>
+      <c r="K39" s="3">
+        <f t="shared" ref="K39" si="37">MAX(K28:K38)</f>
+        <v>5.6918885448916399</v>
+      </c>
+      <c r="L39" s="3">
+        <f t="shared" ref="L39" si="38">MAX(L28:L38)</f>
+        <v>5.7147243107769397</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <f>MAX(B39,B26,B13)</f>
+        <v>3.9799881040662499</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" ref="C41:L41" si="39">MAX(C39,C26,C13)</f>
+        <v>4.37136752136752</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="39"/>
+        <v>4.6829358974359003</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="39"/>
+        <v>4.9005566534914404</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="39"/>
+        <v>5.1330331262940003</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="39"/>
+        <v>5.1990720873329597</v>
+      </c>
+      <c r="H41" s="3">
+        <f t="shared" si="39"/>
+        <v>5.3793939393939398</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" si="39"/>
+        <v>5.5832894736842098</v>
+      </c>
+      <c r="J41" s="3">
+        <f t="shared" si="39"/>
+        <v>5.6094883040935697</v>
+      </c>
+      <c r="K41" s="3">
+        <f t="shared" si="39"/>
+        <v>5.7867905056759597</v>
+      </c>
+      <c r="L41" s="3">
+        <f t="shared" si="39"/>
+        <v>5.8289473684210504</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>10</v>
+      </c>
+      <c r="I42">
+        <v>10</v>
+      </c>
+      <c r="J42">
+        <v>8</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>